<commit_message>
[DOCS]: proffreading analisis economico
</commit_message>
<xml_diff>
--- a/anexos/analisis-economico/analisis-economico.xlsx
+++ b/anexos/analisis-economico/analisis-economico.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ThinkPad\Documents\u\APMG1\Tile-Tech\anexos\analisis-economico\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D94B7AEE-3D83-4E03-B741-68CE3E4CEEB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{974C0D1B-003E-437D-8654-7C595C247372}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="664" activeTab="1" xr2:uid="{F88F103A-AD35-45C9-9307-C4B5E54861C8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="664" activeTab="5" xr2:uid="{F88F103A-AD35-45C9-9307-C4B5E54861C8}"/>
   </bookViews>
   <sheets>
     <sheet name="ACTUAL" sheetId="2" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="189">
   <si>
     <t>PRODUCCION M2</t>
   </si>
@@ -611,6 +611,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>SERVICIOS PÚBLICOS</t>
   </si>
 </sst>
 </file>
@@ -625,10 +628,10 @@
     <numFmt numFmtId="164" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
-    <numFmt numFmtId="168" formatCode="_-&quot;$&quot;\ * #,##0.000_-;\-&quot;$&quot;\ * #,##0.000_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="169" formatCode="_-&quot;$&quot;\ * #,##0.000_-;\-&quot;$&quot;\ * #,##0.000_-;_-&quot;$&quot;\ * &quot;-&quot;???_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="_-&quot;$&quot;\ * #,##0.000_-;\-&quot;$&quot;\ * #,##0.000_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="_-&quot;$&quot;\ * #,##0.000_-;\-&quot;$&quot;\ * #,##0.000_-;_-&quot;$&quot;\ * &quot;-&quot;???_-;_-@_-"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -711,6 +714,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="11">
     <fill>
@@ -1350,7 +1360,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="208">
+  <cellXfs count="210">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1609,6 +1619,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1744,11 +1760,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2104,8 +2116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFAC403C-54EA-4DB7-A3C6-5ABA5B343DBD}">
   <dimension ref="B1:K82"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27:E27"/>
+    <sheetView topLeftCell="A59" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2122,14 +2134,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B1" s="160" t="s">
+      <c r="B1" s="164" t="s">
         <v>105</v>
       </c>
-      <c r="C1" s="160"/>
-      <c r="D1" s="160"/>
-      <c r="E1" s="160"/>
-      <c r="F1" s="160"/>
-      <c r="G1" s="160"/>
+      <c r="C1" s="164"/>
+      <c r="D1" s="164"/>
+      <c r="E1" s="164"/>
+      <c r="F1" s="164"/>
+      <c r="G1" s="164"/>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C2" s="95"/>
@@ -2263,12 +2275,12 @@
       <c r="C17" s="92"/>
     </row>
     <row r="18" spans="2:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="161" t="s">
+      <c r="B18" s="165" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="161"/>
-      <c r="D18" s="161"/>
-      <c r="E18" s="161"/>
+      <c r="C18" s="165"/>
+      <c r="D18" s="165"/>
+      <c r="E18" s="165"/>
     </row>
     <row r="19" spans="2:10" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="79"/>
@@ -2419,12 +2431,12 @@
       <c r="I26" s="140"/>
     </row>
     <row r="27" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="177" t="s">
+      <c r="B27" s="181" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="178"/>
-      <c r="D27" s="178"/>
-      <c r="E27" s="178"/>
+      <c r="C27" s="182"/>
+      <c r="D27" s="182"/>
+      <c r="E27" s="182"/>
       <c r="F27" s="137">
         <f>SUM(F21:F26)</f>
         <v>2339838524.1600003</v>
@@ -2433,12 +2445,12 @@
       <c r="J27" s="134"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B28" s="173" t="s">
-        <v>23</v>
-      </c>
-      <c r="C28" s="173"/>
-      <c r="D28" s="173"/>
-      <c r="E28" s="173"/>
+      <c r="B28" s="177" t="s">
+        <v>188</v>
+      </c>
+      <c r="C28" s="177"/>
+      <c r="D28" s="177"/>
+      <c r="E28" s="177"/>
     </row>
     <row r="29" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B29" s="21" t="s">
@@ -2710,11 +2722,11 @@
       </c>
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B47" s="174" t="s">
+      <c r="B47" s="178" t="s">
         <v>129</v>
       </c>
-      <c r="C47" s="174"/>
-      <c r="D47" s="174"/>
+      <c r="C47" s="178"/>
+      <c r="D47" s="178"/>
       <c r="E47" s="27">
         <f>+E46+E44+E33</f>
         <v>956878960</v>
@@ -2730,22 +2742,22 @@
       <c r="D49" s="13"/>
     </row>
     <row r="50" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="161" t="s">
+      <c r="B50" s="165" t="s">
         <v>6</v>
       </c>
-      <c r="C50" s="161"/>
-      <c r="D50" s="161"/>
-      <c r="E50" s="161"/>
+      <c r="C50" s="165"/>
+      <c r="D50" s="165"/>
+      <c r="E50" s="165"/>
     </row>
     <row r="51" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="174" t="s">
+      <c r="B51" s="178" t="s">
         <v>9</v>
       </c>
-      <c r="C51" s="174"/>
-      <c r="D51" s="174"/>
-      <c r="E51" s="174"/>
-      <c r="F51" s="174"/>
-      <c r="G51" s="174"/>
+      <c r="C51" s="178"/>
+      <c r="D51" s="178"/>
+      <c r="E51" s="178"/>
+      <c r="F51" s="178"/>
+      <c r="G51" s="178"/>
     </row>
     <row r="52" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B52" s="84" t="s">
@@ -2768,7 +2780,7 @@
       </c>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B53" s="167" t="s">
+      <c r="B53" s="171" t="s">
         <v>112</v>
       </c>
       <c r="C53" s="6" t="s">
@@ -2791,7 +2803,7 @@
       </c>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B54" s="168"/>
+      <c r="B54" s="172"/>
       <c r="C54" s="6" t="s">
         <v>116</v>
       </c>
@@ -2812,7 +2824,7 @@
       </c>
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B55" s="168"/>
+      <c r="B55" s="172"/>
       <c r="C55" s="6" t="s">
         <v>117</v>
       </c>
@@ -2833,7 +2845,7 @@
       </c>
     </row>
     <row r="56" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B56" s="168"/>
+      <c r="B56" s="172"/>
       <c r="C56" s="6" t="s">
         <v>118</v>
       </c>
@@ -2854,7 +2866,7 @@
       </c>
     </row>
     <row r="57" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B57" s="168"/>
+      <c r="B57" s="172"/>
       <c r="C57" s="6" t="s">
         <v>119</v>
       </c>
@@ -2875,7 +2887,7 @@
       </c>
     </row>
     <row r="58" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B58" s="168"/>
+      <c r="B58" s="172"/>
       <c r="C58" s="6" t="s">
         <v>120</v>
       </c>
@@ -2896,7 +2908,7 @@
       </c>
     </row>
     <row r="59" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B59" s="168"/>
+      <c r="B59" s="172"/>
       <c r="C59" s="6" t="s">
         <v>101</v>
       </c>
@@ -2917,7 +2929,7 @@
       </c>
     </row>
     <row r="60" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B60" s="169"/>
+      <c r="B60" s="173"/>
       <c r="C60" s="6" t="s">
         <v>21</v>
       </c>
@@ -2936,10 +2948,10 @@
       </c>
     </row>
     <row r="61" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B61" s="175" t="s">
+      <c r="B61" s="179" t="s">
         <v>113</v>
       </c>
-      <c r="C61" s="176"/>
+      <c r="C61" s="180"/>
       <c r="D61" s="6">
         <v>2</v>
       </c>
@@ -2956,11 +2968,11 @@
       </c>
     </row>
     <row r="62" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B62" s="164" t="s">
+      <c r="B62" s="168" t="s">
         <v>114</v>
       </c>
-      <c r="C62" s="165"/>
-      <c r="D62" s="166"/>
+      <c r="C62" s="169"/>
+      <c r="D62" s="170"/>
       <c r="E62" s="35">
         <v>1</v>
       </c>
@@ -2974,13 +2986,13 @@
       </c>
     </row>
     <row r="63" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B63" s="170" t="s">
+      <c r="B63" s="174" t="s">
         <v>21</v>
       </c>
-      <c r="C63" s="171"/>
-      <c r="D63" s="171"/>
-      <c r="E63" s="171"/>
-      <c r="F63" s="171"/>
+      <c r="C63" s="175"/>
+      <c r="D63" s="175"/>
+      <c r="E63" s="175"/>
+      <c r="F63" s="175"/>
       <c r="G63" s="37">
         <f>SUM(G53:G62)</f>
         <v>244296000</v>
@@ -2995,13 +3007,13 @@
       <c r="G64" s="25"/>
     </row>
     <row r="65" spans="2:7" ht="21" x14ac:dyDescent="0.4">
-      <c r="B65" s="162" t="s">
+      <c r="B65" s="166" t="s">
         <v>164</v>
       </c>
-      <c r="C65" s="162"/>
-      <c r="D65" s="162"/>
-      <c r="E65" s="162"/>
-      <c r="F65" s="162"/>
+      <c r="C65" s="166"/>
+      <c r="D65" s="166"/>
+      <c r="E65" s="166"/>
+      <c r="F65" s="166"/>
       <c r="G65" s="25"/>
     </row>
     <row r="66" spans="2:7" x14ac:dyDescent="0.3">
@@ -3013,10 +3025,10 @@
       <c r="G66" s="25"/>
     </row>
     <row r="67" spans="2:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B67" s="163" t="s">
+      <c r="B67" s="167" t="s">
         <v>104</v>
       </c>
-      <c r="C67" s="163"/>
+      <c r="C67" s="167"/>
       <c r="D67" s="7"/>
       <c r="E67" s="7"/>
       <c r="F67" s="7"/>
@@ -3049,10 +3061,10 @@
       <c r="G69" s="25"/>
     </row>
     <row r="70" spans="2:7" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B70" s="172" t="s">
+      <c r="B70" s="176" t="s">
         <v>6</v>
       </c>
-      <c r="C70" s="172"/>
+      <c r="C70" s="176"/>
       <c r="D70" s="7"/>
       <c r="E70" s="7"/>
       <c r="F70" s="7"/>
@@ -3193,8 +3205,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2983426-E21D-4B87-859C-E536AB3C07D4}">
   <dimension ref="B2:L56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="G56" sqref="G56"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3217,32 +3229,32 @@
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="181" t="s">
+      <c r="B4" s="185" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="181"/>
-      <c r="D4" s="181"/>
+      <c r="C4" s="185"/>
+      <c r="D4" s="185"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B5" s="181" t="s">
+      <c r="B5" s="185" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="181"/>
-      <c r="D5" s="181"/>
+      <c r="C5" s="185"/>
+      <c r="D5" s="185"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B6" s="181" t="s">
+      <c r="B6" s="185" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="181"/>
-      <c r="D6" s="181"/>
+      <c r="C6" s="185"/>
+      <c r="D6" s="185"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="181" t="s">
+      <c r="B7" s="185" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="181"/>
-      <c r="D7" s="181"/>
+      <c r="C7" s="185"/>
+      <c r="D7" s="185"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
@@ -3250,35 +3262,35 @@
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="185" t="s">
+      <c r="B11" s="189" t="s">
         <v>136</v>
       </c>
-      <c r="C11" s="185"/>
-      <c r="D11" s="185"/>
-      <c r="E11" s="185"/>
-      <c r="F11" s="185"/>
+      <c r="C11" s="189"/>
+      <c r="D11" s="189"/>
+      <c r="E11" s="189"/>
+      <c r="F11" s="189"/>
     </row>
     <row r="12" spans="2:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="180" t="s">
+      <c r="B12" s="184" t="s">
         <v>137</v>
       </c>
-      <c r="C12" s="180"/>
-      <c r="D12" s="180"/>
-      <c r="E12" s="180"/>
-      <c r="F12" s="180"/>
-      <c r="G12" s="180"/>
-      <c r="H12" s="180"/>
+      <c r="C12" s="184"/>
+      <c r="D12" s="184"/>
+      <c r="E12" s="184"/>
+      <c r="F12" s="184"/>
+      <c r="G12" s="184"/>
+      <c r="H12" s="184"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B14" s="181" t="s">
+      <c r="B14" s="185" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="181"/>
-      <c r="D14" s="181"/>
-      <c r="E14" s="181"/>
-      <c r="F14" s="181"/>
-      <c r="G14" s="181"/>
-      <c r="H14" s="181"/>
+      <c r="C14" s="185"/>
+      <c r="D14" s="185"/>
+      <c r="E14" s="185"/>
+      <c r="F14" s="185"/>
+      <c r="G14" s="185"/>
+      <c r="H14" s="185"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="7"/>
@@ -3290,10 +3302,10 @@
       <c r="H15" s="7"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B16" s="182" t="s">
+      <c r="B16" s="186" t="s">
         <v>138</v>
       </c>
-      <c r="C16" s="182"/>
+      <c r="C16" s="186"/>
       <c r="D16" s="9">
         <v>300000000</v>
       </c>
@@ -3533,10 +3545,10 @@
       </c>
     </row>
     <row r="30" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="186" t="s">
+      <c r="B30" s="190" t="s">
         <v>106</v>
       </c>
-      <c r="C30" s="186"/>
+      <c r="C30" s="190"/>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B31" s="6" t="s">
@@ -3623,10 +3635,10 @@
       <c r="F40" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="G40" s="183" t="s">
+      <c r="G40" s="187" t="s">
         <v>68</v>
       </c>
-      <c r="H40" s="183"/>
+      <c r="H40" s="187"/>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B41" s="15" t="s">
@@ -3645,11 +3657,11 @@
       <c r="F41" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="G41" s="184">
+      <c r="G41" s="188">
         <f>+E41*12</f>
         <v>46800000</v>
       </c>
-      <c r="H41" s="184"/>
+      <c r="H41" s="188"/>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B42" s="15" t="s">
@@ -3663,11 +3675,11 @@
       <c r="F42" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="G42" s="184">
+      <c r="G42" s="188">
         <f t="shared" ref="G42:G44" si="5">+E42*12</f>
         <v>48000000</v>
       </c>
-      <c r="H42" s="184"/>
+      <c r="H42" s="188"/>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B43" s="15" t="s">
@@ -3681,11 +3693,11 @@
       <c r="F43" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="G43" s="184">
+      <c r="G43" s="188">
         <f t="shared" si="5"/>
         <v>24000000</v>
       </c>
-      <c r="H43" s="184"/>
+      <c r="H43" s="188"/>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B44" s="15" t="s">
@@ -3699,11 +3711,11 @@
       <c r="F44" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="G44" s="184">
+      <c r="G44" s="188">
         <f t="shared" si="5"/>
         <v>12000000</v>
       </c>
-      <c r="H44" s="184"/>
+      <c r="H44" s="188"/>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B45" s="51" t="s">
@@ -3713,17 +3725,17 @@
       <c r="D45" s="53"/>
       <c r="E45" s="53"/>
       <c r="F45" s="54"/>
-      <c r="G45" s="179">
+      <c r="G45" s="183">
         <f>SUM(G41:G44)</f>
         <v>130800000</v>
       </c>
-      <c r="H45" s="179"/>
+      <c r="H45" s="183"/>
     </row>
     <row r="47" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="180" t="s">
+      <c r="B47" s="184" t="s">
         <v>109</v>
       </c>
-      <c r="C47" s="180"/>
+      <c r="C47" s="184"/>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B48" s="6" t="s">
@@ -3734,7 +3746,7 @@
         <v>300000000</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B49" s="6" t="s">
         <v>146</v>
       </c>
@@ -3743,7 +3755,7 @@
         <v>1006202255.2435</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B50" s="6" t="s">
         <v>147</v>
       </c>
@@ -3752,7 +3764,7 @@
         <v>260905438.96346474</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B51" s="6" t="s">
         <v>148</v>
       </c>
@@ -3761,7 +3773,7 @@
         <v>130800000</v>
       </c>
     </row>
-    <row r="52" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B52" s="6" t="s">
         <v>21</v>
       </c>
@@ -3770,7 +3782,7 @@
         <v>1267107694.2069647</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B53" s="99" t="s">
         <v>149</v>
       </c>
@@ -3778,7 +3790,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B54" s="6" t="s">
         <v>21</v>
       </c>
@@ -3787,7 +3799,7 @@
         <v>1647240002.4690542</v>
       </c>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B55" s="6" t="s">
         <v>110</v>
       </c>
@@ -3796,13 +3808,17 @@
         <v>329759997.53094578</v>
       </c>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B56" s="17" t="s">
         <v>74</v>
       </c>
       <c r="C56" s="19">
         <f>MROUND(C54*1.2,1000000)</f>
         <v>1977000000</v>
+      </c>
+      <c r="D56" s="163">
+        <f>C55/C56</f>
+        <v>0.16679817781029124</v>
       </c>
     </row>
   </sheetData>
@@ -3834,7 +3850,7 @@
   <dimension ref="B1:N22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B9"/>
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3848,11 +3864,11 @@
       <c r="B1" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="187">
+      <c r="C1" s="191">
         <f>+PROPUESTA!C56</f>
         <v>1977000000</v>
       </c>
-      <c r="D1" s="187"/>
+      <c r="D1" s="191"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
@@ -4116,52 +4132,52 @@
       <c r="B18" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="C18" s="179">
+      <c r="C18" s="183">
         <f>+C16</f>
         <v>395400000</v>
       </c>
-      <c r="D18" s="179"/>
+      <c r="D18" s="183"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B19" s="15" t="s">
         <v>157</v>
       </c>
-      <c r="C19" s="179">
+      <c r="C19" s="183">
         <f>+F16</f>
         <v>395400000</v>
       </c>
-      <c r="D19" s="179"/>
+      <c r="D19" s="183"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B20" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="C20" s="179">
+      <c r="C20" s="183">
         <f>+H16</f>
         <v>395400000</v>
       </c>
-      <c r="D20" s="179"/>
+      <c r="D20" s="183"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B21" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="C21" s="179">
+      <c r="C21" s="183">
         <f>+K16</f>
         <v>593100000</v>
       </c>
-      <c r="D21" s="179"/>
+      <c r="D21" s="183"/>
       <c r="M21" s="2"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B22" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="C22" s="179">
+      <c r="C22" s="183">
         <f>+N16</f>
         <v>197700000</v>
       </c>
-      <c r="D22" s="179"/>
+      <c r="D22" s="183"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -4181,8 +4197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D989884-3E5C-400A-BA14-73D8C7B1295A}">
   <dimension ref="B1:N84"/>
   <sheetViews>
-    <sheetView topLeftCell="A62" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L68" sqref="L68"/>
+    <sheetView topLeftCell="A66" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4198,23 +4214,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B1" s="160" t="s">
+      <c r="B1" s="164" t="s">
         <v>111</v>
       </c>
-      <c r="C1" s="160"/>
-      <c r="D1" s="160"/>
-      <c r="E1" s="160"/>
-      <c r="F1" s="160"/>
-      <c r="G1" s="160"/>
+      <c r="C1" s="164"/>
+      <c r="D1" s="164"/>
+      <c r="E1" s="164"/>
+      <c r="F1" s="164"/>
+      <c r="G1" s="164"/>
     </row>
     <row r="2" spans="2:9" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="188" t="s">
+      <c r="B2" s="192" t="s">
         <v>80</v>
       </c>
-      <c r="C2" s="188"/>
-      <c r="D2" s="188"/>
-      <c r="E2" s="188"/>
-      <c r="F2" s="188"/>
+      <c r="C2" s="192"/>
+      <c r="D2" s="192"/>
+      <c r="E2" s="192"/>
+      <c r="F2" s="192"/>
     </row>
     <row r="5" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B5" s="6"/>
@@ -4346,7 +4362,7 @@
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B13" s="205" t="s">
+      <c r="B13" s="160" t="s">
         <v>125</v>
       </c>
       <c r="C13" s="76">
@@ -4456,12 +4472,12 @@
       <c r="C19" s="50"/>
     </row>
     <row r="20" spans="2:14" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="190" t="s">
+      <c r="B20" s="194" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="190"/>
-      <c r="D20" s="190"/>
-      <c r="E20" s="190"/>
+      <c r="C20" s="194"/>
+      <c r="D20" s="194"/>
+      <c r="E20" s="194"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B21" s="90" t="s">
@@ -4604,24 +4620,24 @@
       </c>
     </row>
     <row r="28" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="177" t="s">
+      <c r="B28" s="181" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="178"/>
-      <c r="D28" s="178"/>
-      <c r="E28" s="178"/>
+      <c r="C28" s="182"/>
+      <c r="D28" s="182"/>
+      <c r="E28" s="182"/>
       <c r="F28" s="137">
         <f>SUM(F22:F27)</f>
         <v>2878001384.7168002</v>
       </c>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B29" s="191" t="s">
+      <c r="B29" s="195" t="s">
         <v>23</v>
       </c>
-      <c r="C29" s="191"/>
-      <c r="D29" s="191"/>
-      <c r="E29" s="191"/>
+      <c r="C29" s="195"/>
+      <c r="D29" s="195"/>
+      <c r="E29" s="195"/>
     </row>
     <row r="30" spans="2:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="21" t="s">
@@ -4904,11 +4920,11 @@
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B48" s="192" t="s">
+      <c r="B48" s="196" t="s">
         <v>33</v>
       </c>
-      <c r="C48" s="193"/>
-      <c r="D48" s="193"/>
+      <c r="C48" s="197"/>
+      <c r="D48" s="197"/>
       <c r="E48" s="25">
         <f>+E47+E45+E34</f>
         <v>1224355480.8</v>
@@ -4918,16 +4934,16 @@
       <c r="D49" s="13"/>
     </row>
     <row r="50" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B50" s="183" t="s">
+      <c r="B50" s="187" t="s">
         <v>9</v>
       </c>
-      <c r="C50" s="183"/>
-      <c r="D50" s="183"/>
-      <c r="E50" s="183"/>
-      <c r="F50" s="183"/>
-      <c r="G50" s="183"/>
-    </row>
-    <row r="51" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C50" s="187"/>
+      <c r="D50" s="187"/>
+      <c r="E50" s="187"/>
+      <c r="F50" s="187"/>
+      <c r="G50" s="187"/>
+    </row>
+    <row r="51" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B51" s="113" t="s">
         <v>34</v>
       </c>
@@ -4948,7 +4964,7 @@
       </c>
     </row>
     <row r="52" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B52" s="167" t="s">
+      <c r="B52" s="171" t="s">
         <v>112</v>
       </c>
       <c r="C52" s="6" t="s">
@@ -4970,7 +4986,7 @@
       </c>
     </row>
     <row r="53" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B53" s="168"/>
+      <c r="B53" s="172"/>
       <c r="C53" s="6" t="s">
         <v>116</v>
       </c>
@@ -4990,7 +5006,7 @@
       </c>
     </row>
     <row r="54" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B54" s="168"/>
+      <c r="B54" s="172"/>
       <c r="C54" s="6" t="s">
         <v>117</v>
       </c>
@@ -5010,7 +5026,7 @@
       </c>
     </row>
     <row r="55" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B55" s="168"/>
+      <c r="B55" s="172"/>
       <c r="C55" s="6" t="s">
         <v>118</v>
       </c>
@@ -5030,7 +5046,7 @@
       </c>
     </row>
     <row r="56" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B56" s="168"/>
+      <c r="B56" s="172"/>
       <c r="C56" s="6" t="s">
         <v>119</v>
       </c>
@@ -5050,7 +5066,7 @@
       </c>
     </row>
     <row r="57" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B57" s="168"/>
+      <c r="B57" s="172"/>
       <c r="C57" s="6" t="s">
         <v>120</v>
       </c>
@@ -5070,7 +5086,7 @@
       </c>
     </row>
     <row r="58" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B58" s="168"/>
+      <c r="B58" s="172"/>
       <c r="C58" s="6" t="s">
         <v>101</v>
       </c>
@@ -5090,7 +5106,7 @@
       </c>
     </row>
     <row r="59" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B59" s="169"/>
+      <c r="B59" s="173"/>
       <c r="C59" s="6" t="s">
         <v>21</v>
       </c>
@@ -5109,10 +5125,10 @@
       </c>
     </row>
     <row r="60" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B60" s="175" t="s">
+      <c r="B60" s="179" t="s">
         <v>113</v>
       </c>
-      <c r="C60" s="176"/>
+      <c r="C60" s="180"/>
       <c r="D60" s="6">
         <v>2</v>
       </c>
@@ -5129,11 +5145,11 @@
       </c>
     </row>
     <row r="61" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B61" s="164" t="s">
+      <c r="B61" s="168" t="s">
         <v>114</v>
       </c>
-      <c r="C61" s="165"/>
-      <c r="D61" s="166"/>
+      <c r="C61" s="169"/>
+      <c r="D61" s="170"/>
       <c r="E61" s="35">
         <v>1</v>
       </c>
@@ -5147,13 +5163,13 @@
       </c>
     </row>
     <row r="62" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B62" s="170" t="s">
+      <c r="B62" s="174" t="s">
         <v>21</v>
       </c>
-      <c r="C62" s="171"/>
-      <c r="D62" s="171"/>
-      <c r="E62" s="171"/>
-      <c r="F62" s="171"/>
+      <c r="C62" s="175"/>
+      <c r="D62" s="175"/>
+      <c r="E62" s="175"/>
+      <c r="F62" s="175"/>
       <c r="G62" s="37">
         <f>SUM(G52:G61)</f>
         <v>159432000</v>
@@ -5166,24 +5182,24 @@
       <c r="E63" s="7"/>
       <c r="F63" s="7"/>
       <c r="G63" s="25"/>
-      <c r="M63" s="206"/>
-      <c r="N63" s="207"/>
+      <c r="M63" s="161"/>
+      <c r="N63" s="162"/>
     </row>
     <row r="64" spans="2:14" ht="21" x14ac:dyDescent="0.4">
-      <c r="B64" s="162" t="s">
+      <c r="B64" s="166" t="s">
         <v>163</v>
       </c>
-      <c r="C64" s="162"/>
-      <c r="D64" s="162"/>
-      <c r="E64" s="162"/>
-      <c r="F64" s="162"/>
+      <c r="C64" s="166"/>
+      <c r="D64" s="166"/>
+      <c r="E64" s="166"/>
+      <c r="F64" s="166"/>
       <c r="G64" s="25"/>
     </row>
     <row r="65" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B65" s="194" t="s">
+      <c r="B65" s="198" t="s">
         <v>104</v>
       </c>
-      <c r="C65" s="194"/>
+      <c r="C65" s="198"/>
       <c r="D65" s="7"/>
       <c r="E65" s="7"/>
       <c r="F65" s="7"/>
@@ -5234,10 +5250,10 @@
       <c r="G68" s="25"/>
     </row>
     <row r="69" spans="2:7" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B69" s="189" t="s">
+      <c r="B69" s="193" t="s">
         <v>6</v>
       </c>
-      <c r="C69" s="189"/>
+      <c r="C69" s="193"/>
       <c r="D69" s="7"/>
       <c r="E69" s="7"/>
       <c r="F69" s="7"/>
@@ -5675,7 +5691,7 @@
         <f>+D10/C10-1</f>
         <v>0.70627870235200474</v>
       </c>
-      <c r="F10" s="195">
+      <c r="F10" s="199">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
@@ -5695,7 +5711,7 @@
         <f t="shared" si="0"/>
         <v>0.36699753414818925</v>
       </c>
-      <c r="F11" s="196"/>
+      <c r="F11" s="200"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" s="105" t="s">
@@ -5713,7 +5729,7 @@
         <f t="shared" si="0"/>
         <v>-6.8574612551533964E-2</v>
       </c>
-      <c r="F12" s="197">
+      <c r="F12" s="201">
         <v>-0.1</v>
       </c>
     </row>
@@ -5733,7 +5749,7 @@
         <f t="shared" si="0"/>
         <v>-6.8574612551533853E-2</v>
       </c>
-      <c r="F13" s="198"/>
+      <c r="F13" s="202"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -5753,11 +5769,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BADFFA1A-762C-454E-8EB2-63C69813CEF7}">
   <dimension ref="B1:AB32"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="7" topLeftCell="D23" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="3" ySplit="7" topLeftCell="D24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="D37" sqref="D37"/>
+      <selection pane="bottomRight" activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5786,30 +5802,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="D1" s="199" t="s">
+      <c r="D1" s="203" t="s">
         <v>161</v>
       </c>
-      <c r="E1" s="199"/>
-      <c r="F1" s="199"/>
-      <c r="G1" s="199"/>
-      <c r="J1" s="199" t="s">
+      <c r="E1" s="203"/>
+      <c r="F1" s="203"/>
+      <c r="G1" s="203"/>
+      <c r="J1" s="203" t="s">
         <v>161</v>
       </c>
-      <c r="K1" s="199"/>
-      <c r="L1" s="199"/>
-      <c r="M1" s="199"/>
-      <c r="P1" s="199" t="s">
+      <c r="K1" s="203"/>
+      <c r="L1" s="203"/>
+      <c r="M1" s="203"/>
+      <c r="P1" s="203" t="s">
         <v>161</v>
       </c>
-      <c r="Q1" s="199"/>
-      <c r="R1" s="199"/>
-      <c r="S1" s="199"/>
-      <c r="W1" s="199" t="s">
+      <c r="Q1" s="203"/>
+      <c r="R1" s="203"/>
+      <c r="S1" s="203"/>
+      <c r="W1" s="203" t="s">
         <v>161</v>
       </c>
-      <c r="X1" s="199"/>
-      <c r="Y1" s="199"/>
-      <c r="Z1" s="199"/>
+      <c r="X1" s="203"/>
+      <c r="Y1" s="203"/>
+      <c r="Z1" s="203"/>
     </row>
     <row r="2" spans="2:28" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C2" s="1" t="s">
@@ -5821,37 +5837,37 @@
       <c r="J2" s="80">
         <v>0.5</v>
       </c>
-      <c r="M2" s="181" t="s">
+      <c r="M2" s="185" t="s">
         <v>91</v>
       </c>
-      <c r="N2" s="181"/>
-      <c r="O2" s="181"/>
+      <c r="N2" s="185"/>
+      <c r="O2" s="185"/>
       <c r="W2" s="112"/>
     </row>
     <row r="3" spans="2:28" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C3" s="1"/>
       <c r="D3" s="2"/>
-      <c r="J3" s="200" t="s">
+      <c r="J3" s="204" t="s">
         <v>168</v>
       </c>
-      <c r="K3" s="200"/>
+      <c r="K3" s="204"/>
       <c r="M3" s="128" t="s">
         <v>165</v>
       </c>
       <c r="N3" s="128" t="s">
         <v>166</v>
       </c>
-      <c r="O3" s="200"/>
-      <c r="P3" s="200"/>
+      <c r="O3" s="204"/>
+      <c r="P3" s="204"/>
       <c r="W3" s="129" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="4" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B4" s="183" t="s">
+      <c r="B4" s="187" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="183"/>
+      <c r="C4" s="187"/>
       <c r="D4" s="6">
         <v>0</v>
       </c>
@@ -5929,10 +5945,10 @@
       </c>
     </row>
     <row r="5" spans="2:28" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="203" t="s">
+      <c r="B5" s="207" t="s">
         <v>167</v>
       </c>
-      <c r="C5" s="204"/>
+      <c r="C5" s="208"/>
       <c r="D5" s="41">
         <v>1</v>
       </c>
@@ -6010,10 +6026,10 @@
       </c>
     </row>
     <row r="6" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B6" s="182" t="s">
+      <c r="B6" s="186" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="182"/>
+      <c r="C6" s="186"/>
       <c r="D6" s="26">
         <f>+INT(ACTUAL!$C$11)*D5</f>
         <v>190564</v>
@@ -6116,10 +6132,10 @@
       </c>
     </row>
     <row r="7" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B7" s="202" t="s">
+      <c r="B7" s="206" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="202"/>
+      <c r="C7" s="206"/>
       <c r="D7" s="108">
         <f>+ACTUAL!C16</f>
         <v>5399800560</v>
@@ -6222,7 +6238,7 @@
       </c>
     </row>
     <row r="8" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B8" s="201" t="s">
+      <c r="B8" s="205" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="6" t="s">
@@ -6330,7 +6346,7 @@
       </c>
     </row>
     <row r="9" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B9" s="201"/>
+      <c r="B9" s="205"/>
       <c r="C9" s="6" t="s">
         <v>8</v>
       </c>
@@ -6436,7 +6452,7 @@
       </c>
     </row>
     <row r="10" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B10" s="201"/>
+      <c r="B10" s="205"/>
       <c r="C10" s="6" t="s">
         <v>15</v>
       </c>
@@ -6542,7 +6558,7 @@
       </c>
     </row>
     <row r="11" spans="2:28" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B11" s="201"/>
+      <c r="B11" s="205"/>
       <c r="C11" s="15" t="s">
         <v>10</v>
       </c>
@@ -6648,7 +6664,7 @@
       </c>
     </row>
     <row r="12" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B12" s="201"/>
+      <c r="B12" s="205"/>
       <c r="C12" s="6" t="s">
         <v>11</v>
       </c>
@@ -6754,7 +6770,7 @@
       </c>
     </row>
     <row r="13" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B13" s="201"/>
+      <c r="B13" s="205"/>
       <c r="C13" s="6" t="s">
         <v>84</v>
       </c>
@@ -6860,7 +6876,7 @@
       </c>
     </row>
     <row r="14" spans="2:28" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="B14" s="201"/>
+      <c r="B14" s="205"/>
       <c r="C14" s="110" t="s">
         <v>13</v>
       </c>
@@ -8004,7 +8020,7 @@
       <c r="C31" t="s">
         <v>171</v>
       </c>
-      <c r="D31" s="5">
+      <c r="D31" s="209">
         <f>+D27</f>
         <v>-395400000</v>
       </c>

</xml_diff>